<commit_message>
FHIR 4.3.0, some fixes
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-lab-observation.xlsx
+++ b/output/StructureDefinition-lab-observation.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1842" uniqueCount="366">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-10-25T15:37:55+02:00</t>
+    <t>2022-10-26T12:16:30+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -78,7 +78,7 @@
     <t>FHIR Version</t>
   </si>
   <si>
-    <t>4.0.1</t>
+    <t>4.3.0</t>
   </si>
   <si>
     <t>Kind</t>
@@ -254,6 +254,9 @@
     <t>Observation[classCode=OBS, moodCode=DEF]</t>
   </si>
   <si>
+    <t>clinical.diagnostics</t>
+  </si>
+  <si>
     <t>Test</t>
   </si>
   <si>
@@ -340,7 +343,7 @@
     <t>preferred</t>
   </si>
   <si>
-    <t>A human language.</t>
+    <t>IETF language tag</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/ValueSet/languages</t>
@@ -398,6 +401,10 @@
     <t>DomainResource.contained</t>
   </si>
   <si>
+    <t xml:space="preserve">dom-r4b:Containing new R4B resources within R4 resources may cause interoperability issues if instances are shared with R4 systems {($this is Citation or $this is Evidence or $this is EvidenceReport or $this is EvidenceVariable or $this is MedicinalProductDefinition or $this is PackagedProductDefinition or $this is AdministrableProductDefinition or $this is Ingredient or $this is ClinicalUseDefinition or $this is RegulatedAuthorization or $this is SubstanceDefinition or $this is SubscriptionStatus or $this is SubscriptionTopic) implies (%resource is Citation or %resource is Evidence or %resource is EvidenceReport or %resource is EvidenceVariable or %resource is MedicinalProductDefinition or %resource is PackagedProductDefinition or %resource is AdministrableProductDefinition or %resource is Ingredient or %resource is ClinicalUseDefinition or %resource is RegulatedAuthorization or %resource is SubstanceDefinition or %resource is SubscriptionStatus or %resource is SubscriptionTopic)}
+</t>
+  </si>
+  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -438,7 +445,7 @@
 Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
   </si>
   <si>
-    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
+    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/2021Mar/extensibility.html#modifierExtension).</t>
   </si>
   <si>
     <t>DomainResource.modifierExtension</t>
@@ -517,102 +524,102 @@
     <t>ObservationDefinition.code.id</t>
   </si>
   <si>
+    <t>Unique id for inter-element referencing</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>ObservationDefinition.code.extension</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
+  </si>
+  <si>
+    <t>ObservationDefinition.code.coding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coding
+</t>
+  </si>
+  <si>
+    <t>Code defined by a terminology system</t>
+  </si>
+  <si>
+    <t>A reference to a code defined by a terminology system.</t>
+  </si>
+  <si>
+    <t>Codes may be defined very casually in enumerations, or code lists, up to very formal definitions such as SNOMED CT - see the HL7 v3 Core Principles for more information.  Ordering of codings is undefined and SHALL NOT be used to infer meaning. Generally, at most only one of the coding values will be labeled as UserSelected = true.</t>
+  </si>
+  <si>
+    <t>Allows for alternative encodings within a code system, and translations to other code systems.</t>
+  </si>
+  <si>
+    <t>CodeableConcept.coding</t>
+  </si>
+  <si>
+    <t>C*E.1-8, C*E.10-22</t>
+  </si>
+  <si>
+    <t>union(., ./translation)</t>
+  </si>
+  <si>
+    <t>ObservationDefinition.code.coding.id</t>
+  </si>
+  <si>
+    <t>ObservationDefinition.code.coding.extension</t>
+  </si>
+  <si>
+    <t>ObservationDefinition.code.coding.system</t>
+  </si>
+  <si>
+    <t>Identity of the terminology system</t>
+  </si>
+  <si>
+    <t>The identification of the code system that defines the meaning of the symbol in the code.</t>
+  </si>
+  <si>
+    <t>The URI may be an OID (urn:oid:...) or a UUID (urn:uuid:...).  OIDs and UUIDs SHALL be references to the HL7 OID registry. Otherwise, the URI should come from HL7's list of FHIR defined special URIs or it should reference to some definition that establishes the system clearly and unambiguously.</t>
+  </si>
+  <si>
+    <t>Need to be unambiguous about the source of the definition of the symbol.</t>
+  </si>
+  <si>
+    <t>Coding.system</t>
+  </si>
+  <si>
+    <t>C*E.3</t>
+  </si>
+  <si>
+    <t>./codeSystem</t>
+  </si>
+  <si>
+    <t>ObservationDefinition.code.coding.version</t>
+  </si>
+  <si>
     <t xml:space="preserve">string
 </t>
   </si>
   <si>
-    <t>Unique id for inter-element referencing</t>
-  </si>
-  <si>
-    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
-  </si>
-  <si>
-    <t>Element.id</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
-    <t>ObservationDefinition.code.extension</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:url}
-</t>
-  </si>
-  <si>
-    <t>Extensions are always sliced by (at least) url</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
-    <t>Element.extension</t>
-  </si>
-  <si>
-    <t>ObservationDefinition.code.coding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coding
-</t>
-  </si>
-  <si>
-    <t>Code defined by a terminology system</t>
-  </si>
-  <si>
-    <t>A reference to a code defined by a terminology system.</t>
-  </si>
-  <si>
-    <t>Codes may be defined very casually in enumerations, or code lists, up to very formal definitions such as SNOMED CT - see the HL7 v3 Core Principles for more information.  Ordering of codings is undefined and SHALL NOT be used to infer meaning. Generally, at most only one of the coding values will be labeled as UserSelected = true.</t>
-  </si>
-  <si>
-    <t>Allows for alternative encodings within a code system, and translations to other code systems.</t>
-  </si>
-  <si>
-    <t>CodeableConcept.coding</t>
-  </si>
-  <si>
-    <t>C*E.1-8, C*E.10-22</t>
-  </si>
-  <si>
-    <t>union(., ./translation)</t>
-  </si>
-  <si>
-    <t>ObservationDefinition.code.coding.id</t>
-  </si>
-  <si>
-    <t>ObservationDefinition.code.coding.extension</t>
-  </si>
-  <si>
-    <t>ObservationDefinition.code.coding.system</t>
-  </si>
-  <si>
-    <t>Identity of the terminology system</t>
-  </si>
-  <si>
-    <t>The identification of the code system that defines the meaning of the symbol in the code.</t>
-  </si>
-  <si>
-    <t>The URI may be an OID (urn:oid:...) or a UUID (urn:uuid:...).  OIDs and UUIDs SHALL be references to the HL7 OID registry. Otherwise, the URI should come from HL7's list of FHIR defined special URIs or it should reference to some definition that establishes the system clearly and unambiguously.</t>
-  </si>
-  <si>
-    <t>Need to be unambiguous about the source of the definition of the symbol.</t>
-  </si>
-  <si>
-    <t>Coding.system</t>
-  </si>
-  <si>
-    <t>C*E.3</t>
-  </si>
-  <si>
-    <t>./codeSystem</t>
-  </si>
-  <si>
-    <t>ObservationDefinition.code.coding.version</t>
-  </si>
-  <si>
     <t>Version of the system - if relevant</t>
   </si>
   <si>
@@ -762,7 +769,7 @@
     <t>Permitted data type for observation value.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/permitted-data-type|4.0.1</t>
+    <t>http://hl7.org/fhir/ValueSet/permitted-data-type|4.3.0</t>
   </si>
   <si>
     <t>OM1-3</t>
@@ -835,6 +842,10 @@
     <t>Characteristics for quantitative results of this observation.</t>
   </si>
   <si>
+    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children unless an empty Parameters resource {hasValue() or (children().count() &gt; id.count()) or $this is Parameters}
+</t>
+  </si>
+  <si>
     <t>OM2</t>
   </si>
   <si>
@@ -962,7 +973,7 @@
     <t>Codes identifying the category of observation range.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/observation-range-category|4.0.1</t>
+    <t>http://hl7.org/fhir/ValueSet/observation-range-category|4.3.0</t>
   </si>
   <si>
     <t>OM-2</t>
@@ -1038,7 +1049,7 @@
     <t>The gender of a person used for administrative purposes.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/administrative-gender|4.0.1</t>
+    <t>http://hl7.org/fhir/ValueSet/administrative-gender|4.3.0</t>
   </si>
   <si>
     <t>RFR.2</t>
@@ -1693,15 +1704,15 @@
         <v>78</v>
       </c>
       <c r="AL2" t="s" s="2">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="AM2" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s" s="2">
@@ -1712,7 +1723,7 @@
         <v>72</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G3" t="s" s="2">
         <v>71</v>
@@ -1721,19 +1732,19 @@
         <v>71</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M3" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" t="s" s="2">
@@ -1783,13 +1794,13 @@
         <v>71</v>
       </c>
       <c r="AE3" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AF3" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG3" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH3" t="s" s="2">
         <v>71</v>
@@ -1812,7 +1823,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
@@ -1823,7 +1834,7 @@
         <v>72</v>
       </c>
       <c r="F4" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G4" t="s" s="2">
         <v>71</v>
@@ -1832,16 +1843,16 @@
         <v>71</v>
       </c>
       <c r="I4" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -1892,19 +1903,19 @@
         <v>71</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AF4" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG4" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH4" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ4" t="s" s="2">
         <v>71</v>
@@ -1921,7 +1932,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -1932,28 +1943,28 @@
         <v>72</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G5" t="s" s="2">
         <v>71</v>
       </c>
       <c r="H5" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
@@ -2003,19 +2014,19 @@
         <v>71</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AF5" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG5" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH5" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ5" t="s" s="2">
         <v>71</v>
@@ -2032,7 +2043,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -2043,7 +2054,7 @@
         <v>72</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G6" t="s" s="2">
         <v>71</v>
@@ -2055,16 +2066,16 @@
         <v>71</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" t="s" s="2">
@@ -2090,13 +2101,13 @@
         <v>71</v>
       </c>
       <c r="W6" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="X6" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="Y6" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="Z6" t="s" s="2">
         <v>71</v>
@@ -2114,19 +2125,19 @@
         <v>71</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="AF6" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG6" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH6" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ6" t="s" s="2">
         <v>71</v>
@@ -2143,18 +2154,18 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s" s="2">
         <v>72</v>
       </c>
       <c r="F7" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G7" t="s" s="2">
         <v>71</v>
@@ -2166,16 +2177,16 @@
         <v>71</v>
       </c>
       <c r="J7" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" t="s" s="2">
@@ -2225,25 +2236,25 @@
         <v>71</v>
       </c>
       <c r="AE7" t="s" s="2">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AF7" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG7" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH7" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI7" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ7" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AK7" t="s" s="2">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AL7" t="s" s="2">
         <v>71</v>
@@ -2254,11 +2265,11 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" t="s" s="2">
@@ -2277,16 +2288,16 @@
         <v>71</v>
       </c>
       <c r="J8" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" t="s" s="2">
@@ -2336,7 +2347,7 @@
         <v>71</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AF8" t="s" s="2">
         <v>72</v>
@@ -2348,13 +2359,13 @@
         <v>71</v>
       </c>
       <c r="AI8" t="s" s="2">
-        <v>71</v>
+        <v>125</v>
       </c>
       <c r="AJ8" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AK8" t="s" s="2">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="AL8" t="s" s="2">
         <v>71</v>
@@ -2365,11 +2376,11 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s" s="2">
@@ -2388,16 +2399,16 @@
         <v>71</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
@@ -2447,7 +2458,7 @@
         <v>71</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="AF9" t="s" s="2">
         <v>72</v>
@@ -2459,13 +2470,13 @@
         <v>71</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="AJ9" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AK9" t="s" s="2">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="AL9" t="s" s="2">
         <v>71</v>
@@ -2476,11 +2487,11 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s" s="2">
@@ -2493,25 +2504,25 @@
         <v>71</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I10" t="s" s="2">
         <v>71</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="N10" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="O10" t="s" s="2">
         <v>71</v>
@@ -2560,7 +2571,7 @@
         <v>71</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>72</v>
@@ -2572,13 +2583,13 @@
         <v>71</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="AJ10" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AK10" t="s" s="2">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="AL10" t="s" s="2">
         <v>71</v>
@@ -2589,11 +2600,11 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
@@ -2609,22 +2620,22 @@
         <v>71</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="N11" t="s" s="2">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="O11" t="s" s="2">
         <v>71</v>
@@ -2649,13 +2660,13 @@
         <v>71</v>
       </c>
       <c r="W11" t="s" s="2">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="X11" t="s" s="2">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="Y11" t="s" s="2">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="Z11" t="s" s="2">
         <v>71</v>
@@ -2673,7 +2684,7 @@
         <v>71</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>72</v>
@@ -2685,16 +2696,16 @@
         <v>71</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ11" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="AM11" t="s" s="2">
         <v>71</v>
@@ -2702,18 +2713,18 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G12" t="s" s="2">
         <v>71</v>
@@ -2722,20 +2733,20 @@
         <v>71</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" t="s" s="2">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="O12" t="s" s="2">
         <v>71</v>
@@ -2760,13 +2771,13 @@
         <v>71</v>
       </c>
       <c r="W12" t="s" s="2">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="X12" t="s" s="2">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="Y12" t="s" s="2">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="Z12" t="s" s="2">
         <v>71</v>
@@ -2784,28 +2795,28 @@
         <v>71</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AG12" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH12" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="AM12" t="s" s="2">
         <v>71</v>
@@ -2813,7 +2824,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -2824,7 +2835,7 @@
         <v>72</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G13" t="s" s="2">
         <v>71</v>
@@ -2836,13 +2847,13 @@
         <v>71</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>161</v>
+        <v>84</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -2893,13 +2904,13 @@
         <v>71</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG13" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH13" t="s" s="2">
         <v>71</v>
@@ -2911,7 +2922,7 @@
         <v>71</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AL13" t="s" s="2">
         <v>71</v>
@@ -2922,11 +2933,11 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
@@ -2945,16 +2956,16 @@
         <v>71</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
@@ -2992,19 +3003,19 @@
         <v>71</v>
       </c>
       <c r="AA14" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AB14" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AC14" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AD14" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>72</v>
@@ -3016,13 +3027,13 @@
         <v>71</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="AJ14" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AL14" t="s" s="2">
         <v>71</v>
@@ -3033,7 +3044,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -3053,22 +3064,22 @@
         <v>71</v>
       </c>
       <c r="I15" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="N15" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="O15" t="s" s="2">
         <v>71</v>
@@ -3117,7 +3128,7 @@
         <v>71</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>72</v>
@@ -3129,13 +3140,13 @@
         <v>71</v>
       </c>
       <c r="AI15" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="AL15" t="s" s="2">
         <v>71</v>
@@ -3146,7 +3157,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -3157,7 +3168,7 @@
         <v>72</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G16" t="s" s="2">
         <v>71</v>
@@ -3169,13 +3180,13 @@
         <v>71</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>161</v>
+        <v>84</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -3226,13 +3237,13 @@
         <v>71</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG16" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH16" t="s" s="2">
         <v>71</v>
@@ -3244,7 +3255,7 @@
         <v>71</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AL16" t="s" s="2">
         <v>71</v>
@@ -3255,11 +3266,11 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
@@ -3278,16 +3289,16 @@
         <v>71</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" t="s" s="2">
@@ -3325,19 +3336,19 @@
         <v>71</v>
       </c>
       <c r="AA17" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AB17" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AC17" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AD17" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>72</v>
@@ -3349,13 +3360,13 @@
         <v>71</v>
       </c>
       <c r="AI17" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="AJ17" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AL17" t="s" s="2">
         <v>71</v>
@@ -3366,7 +3377,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3377,7 +3388,7 @@
         <v>72</v>
       </c>
       <c r="F18" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G18" t="s" s="2">
         <v>71</v>
@@ -3386,22 +3397,22 @@
         <v>71</v>
       </c>
       <c r="I18" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="O18" t="s" s="2">
         <v>71</v>
@@ -3450,25 +3461,25 @@
         <v>71</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG18" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH18" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI18" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AL18" t="s" s="2">
         <v>71</v>
@@ -3479,7 +3490,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3490,7 +3501,7 @@
         <v>72</v>
       </c>
       <c r="F19" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G19" t="s" s="2">
         <v>71</v>
@@ -3499,19 +3510,19 @@
         <v>71</v>
       </c>
       <c r="I19" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>161</v>
+        <v>193</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
@@ -3561,25 +3572,25 @@
         <v>71</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG19" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH19" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>71</v>
@@ -3590,7 +3601,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3601,7 +3612,7 @@
         <v>72</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G20" t="s" s="2">
         <v>71</v>
@@ -3610,20 +3621,20 @@
         <v>71</v>
       </c>
       <c r="I20" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" t="s" s="2">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>71</v>
@@ -3672,36 +3683,36 @@
         <v>71</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG20" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH20" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="AL20" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3712,7 +3723,7 @@
         <v>72</v>
       </c>
       <c r="F21" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G21" t="s" s="2">
         <v>71</v>
@@ -3721,20 +3732,20 @@
         <v>71</v>
       </c>
       <c r="I21" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>161</v>
+        <v>193</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" t="s" s="2">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>71</v>
@@ -3783,36 +3794,36 @@
         <v>71</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG21" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH21" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="AL21" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3823,7 +3834,7 @@
         <v>72</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G22" t="s" s="2">
         <v>71</v>
@@ -3832,22 +3843,22 @@
         <v>71</v>
       </c>
       <c r="I22" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>71</v>
@@ -3896,25 +3907,25 @@
         <v>71</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG22" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH22" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="AL22" t="s" s="2">
         <v>71</v>
@@ -3925,7 +3936,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3936,7 +3947,7 @@
         <v>72</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>71</v>
@@ -3945,22 +3956,22 @@
         <v>71</v>
       </c>
       <c r="I23" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>161</v>
+        <v>193</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>71</v>
@@ -4009,25 +4020,25 @@
         <v>71</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH23" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>71</v>
@@ -4038,7 +4049,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4058,16 +4069,16 @@
         <v>71</v>
       </c>
       <c r="I24" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -4118,7 +4129,7 @@
         <v>71</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>72</v>
@@ -4130,7 +4141,7 @@
         <v>71</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ24" t="s" s="2">
         <v>71</v>
@@ -4147,7 +4158,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4170,13 +4181,13 @@
         <v>71</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -4191,7 +4202,7 @@
         <v>71</v>
       </c>
       <c r="S25" t="s" s="2">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="T25" t="s" s="2">
         <v>71</v>
@@ -4203,13 +4214,13 @@
         <v>71</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>71</v>
@@ -4227,7 +4238,7 @@
         <v>71</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>72</v>
@@ -4239,10 +4250,10 @@
         <v>71</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="AK25" t="s" s="2">
         <v>71</v>
@@ -4256,7 +4267,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4267,7 +4278,7 @@
         <v>72</v>
       </c>
       <c r="F26" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G26" t="s" s="2">
         <v>71</v>
@@ -4279,16 +4290,16 @@
         <v>71</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
@@ -4302,7 +4313,7 @@
         <v>71</v>
       </c>
       <c r="S26" t="s" s="2">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="T26" t="s" s="2">
         <v>71</v>
@@ -4338,19 +4349,19 @@
         <v>71</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG26" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH26" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ26" t="s" s="2">
         <v>71</v>
@@ -4367,7 +4378,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4378,7 +4389,7 @@
         <v>72</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G27" t="s" s="2">
         <v>71</v>
@@ -4390,19 +4401,19 @@
         <v>71</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>71</v>
@@ -4427,13 +4438,13 @@
         <v>71</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>71</v>
@@ -4451,25 +4462,25 @@
         <v>71</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG27" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH27" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI27" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>71</v>
@@ -4480,7 +4491,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4491,7 +4502,7 @@
         <v>72</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G28" t="s" s="2">
         <v>71</v>
@@ -4503,13 +4514,13 @@
         <v>71</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>161</v>
+        <v>193</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -4560,22 +4571,22 @@
         <v>71</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG28" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH28" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI28" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>71</v>
@@ -4589,7 +4600,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4600,7 +4611,7 @@
         <v>72</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>71</v>
@@ -4612,13 +4623,13 @@
         <v>71</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -4669,22 +4680,22 @@
         <v>71</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG29" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH29" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>93</v>
+        <v>267</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="AK29" t="s" s="2">
         <v>71</v>
@@ -4698,7 +4709,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4709,7 +4720,7 @@
         <v>72</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G30" t="s" s="2">
         <v>71</v>
@@ -4721,13 +4732,13 @@
         <v>71</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>161</v>
+        <v>193</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -4778,13 +4789,13 @@
         <v>71</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG30" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH30" t="s" s="2">
         <v>71</v>
@@ -4796,7 +4807,7 @@
         <v>71</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>71</v>
@@ -4807,11 +4818,11 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" t="s" s="2">
@@ -4830,16 +4841,16 @@
         <v>71</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -4889,7 +4900,7 @@
         <v>71</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>72</v>
@@ -4901,13 +4912,13 @@
         <v>71</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="AJ31" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>71</v>
@@ -4918,11 +4929,11 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
@@ -4935,25 +4946,25 @@
         <v>71</v>
       </c>
       <c r="H32" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>71</v>
@@ -5002,7 +5013,7 @@
         <v>71</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>72</v>
@@ -5014,13 +5025,13 @@
         <v>71</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="AJ32" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="AL32" t="s" s="2">
         <v>71</v>
@@ -5031,7 +5042,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5042,7 +5053,7 @@
         <v>72</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>71</v>
@@ -5054,13 +5065,13 @@
         <v>71</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -5087,46 +5098,46 @@
         <v>71</v>
       </c>
       <c r="W33" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="X33" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="Y33" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="Z33" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AA33" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AB33" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AC33" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AD33" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AE33" t="s" s="2">
         <v>276</v>
       </c>
-      <c r="X33" t="s" s="2">
-        <v>277</v>
-      </c>
-      <c r="Y33" t="s" s="2">
-        <v>278</v>
-      </c>
-      <c r="Z33" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AA33" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AB33" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AC33" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AD33" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AE33" t="s" s="2">
-        <v>273</v>
-      </c>
       <c r="AF33" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH33" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="AK33" t="s" s="2">
         <v>71</v>
@@ -5140,7 +5151,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5151,7 +5162,7 @@
         <v>72</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G34" t="s" s="2">
         <v>71</v>
@@ -5163,13 +5174,13 @@
         <v>71</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -5196,13 +5207,13 @@
         <v>71</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="X34" t="s" s="2">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>71</v>
@@ -5220,22 +5231,22 @@
         <v>71</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG34" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH34" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI34" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>71</v>
@@ -5249,7 +5260,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5260,7 +5271,7 @@
         <v>72</v>
       </c>
       <c r="F35" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G35" t="s" s="2">
         <v>71</v>
@@ -5272,13 +5283,13 @@
         <v>71</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5329,22 +5340,22 @@
         <v>71</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG35" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH35" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>71</v>
@@ -5358,7 +5369,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5369,7 +5380,7 @@
         <v>72</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>71</v>
@@ -5381,13 +5392,13 @@
         <v>71</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5438,22 +5449,22 @@
         <v>71</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG36" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH36" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>71</v>
@@ -5467,7 +5478,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5490,13 +5501,13 @@
         <v>71</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -5547,7 +5558,7 @@
         <v>71</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>72</v>
@@ -5559,10 +5570,10 @@
         <v>71</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>93</v>
+        <v>267</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>71</v>
@@ -5576,7 +5587,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5587,7 +5598,7 @@
         <v>72</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G38" t="s" s="2">
         <v>71</v>
@@ -5599,13 +5610,13 @@
         <v>71</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>161</v>
+        <v>193</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
@@ -5656,13 +5667,13 @@
         <v>71</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG38" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH38" t="s" s="2">
         <v>71</v>
@@ -5674,7 +5685,7 @@
         <v>71</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AL38" t="s" s="2">
         <v>71</v>
@@ -5685,11 +5696,11 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
@@ -5708,16 +5719,16 @@
         <v>71</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
@@ -5767,7 +5778,7 @@
         <v>71</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>72</v>
@@ -5779,13 +5790,13 @@
         <v>71</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="AJ39" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>71</v>
@@ -5796,11 +5807,11 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" t="s" s="2">
@@ -5813,25 +5824,25 @@
         <v>71</v>
       </c>
       <c r="H40" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I40" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>71</v>
@@ -5880,7 +5891,7 @@
         <v>71</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>72</v>
@@ -5892,13 +5903,13 @@
         <v>71</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="AJ40" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>71</v>
@@ -5909,7 +5920,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5920,7 +5931,7 @@
         <v>72</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>71</v>
@@ -5932,13 +5943,13 @@
         <v>71</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -5953,58 +5964,58 @@
         <v>71</v>
       </c>
       <c r="S41" t="s" s="2">
+        <v>307</v>
+      </c>
+      <c r="T41" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="U41" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="V41" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="W41" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="X41" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="Y41" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="Z41" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AA41" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AB41" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AC41" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AD41" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AE41" t="s" s="2">
         <v>304</v>
       </c>
-      <c r="T41" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="U41" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="V41" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="W41" t="s" s="2">
-        <v>239</v>
-      </c>
-      <c r="X41" t="s" s="2">
-        <v>305</v>
-      </c>
-      <c r="Y41" t="s" s="2">
-        <v>306</v>
-      </c>
-      <c r="Z41" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AA41" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AB41" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AC41" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AD41" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AE41" t="s" s="2">
-        <v>301</v>
-      </c>
       <c r="AF41" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="AK41" t="s" s="2">
         <v>71</v>
@@ -6018,7 +6029,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6029,7 +6040,7 @@
         <v>72</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>71</v>
@@ -6041,17 +6052,17 @@
         <v>71</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" t="s" s="2">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="O42" t="s" s="2">
         <v>71</v>
@@ -6100,22 +6111,22 @@
         <v>71</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG42" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH42" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="AK42" t="s" s="2">
         <v>71</v>
@@ -6129,7 +6140,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6140,7 +6151,7 @@
         <v>72</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>71</v>
@@ -6152,13 +6163,13 @@
         <v>71</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
@@ -6185,46 +6196,46 @@
         <v>71</v>
       </c>
       <c r="W43" t="s" s="2">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="X43" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="Y43" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="Z43" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AA43" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AB43" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AC43" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AD43" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AE43" t="s" s="2">
         <v>316</v>
       </c>
-      <c r="Y43" t="s" s="2">
-        <v>317</v>
-      </c>
-      <c r="Z43" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AA43" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AB43" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AC43" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AD43" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AE43" t="s" s="2">
-        <v>313</v>
-      </c>
       <c r="AF43" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH43" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="AK43" t="s" s="2">
         <v>71</v>
@@ -6238,7 +6249,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6261,16 +6272,16 @@
         <v>71</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
@@ -6296,13 +6307,13 @@
         <v>71</v>
       </c>
       <c r="W44" t="s" s="2">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="Z44" t="s" s="2">
         <v>71</v>
@@ -6320,7 +6331,7 @@
         <v>71</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>72</v>
@@ -6332,10 +6343,10 @@
         <v>71</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="AK44" t="s" s="2">
         <v>71</v>
@@ -6349,7 +6360,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6360,7 +6371,7 @@
         <v>72</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>71</v>
@@ -6372,13 +6383,13 @@
         <v>71</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -6393,58 +6404,58 @@
         <v>71</v>
       </c>
       <c r="S45" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="T45" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="U45" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="V45" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="W45" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="X45" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="Y45" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="Z45" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AA45" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AB45" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AC45" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AD45" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="AE45" t="s" s="2">
         <v>329</v>
       </c>
-      <c r="T45" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="U45" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="V45" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="W45" t="s" s="2">
-        <v>239</v>
-      </c>
-      <c r="X45" t="s" s="2">
-        <v>330</v>
-      </c>
-      <c r="Y45" t="s" s="2">
-        <v>331</v>
-      </c>
-      <c r="Z45" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AA45" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AB45" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AC45" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AD45" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="AE45" t="s" s="2">
-        <v>326</v>
-      </c>
       <c r="AF45" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH45" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>71</v>
@@ -6458,7 +6469,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6469,7 +6480,7 @@
         <v>72</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>71</v>
@@ -6481,16 +6492,16 @@
         <v>71</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
@@ -6540,22 +6551,22 @@
         <v>71</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG46" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH46" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="AK46" t="s" s="2">
         <v>71</v>
@@ -6569,7 +6580,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6580,7 +6591,7 @@
         <v>72</v>
       </c>
       <c r="F47" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G47" t="s" s="2">
         <v>71</v>
@@ -6592,13 +6603,13 @@
         <v>71</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -6649,22 +6660,22 @@
         <v>71</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG47" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH47" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="AK47" t="s" s="2">
         <v>71</v>
@@ -6678,7 +6689,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6689,7 +6700,7 @@
         <v>72</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G48" t="s" s="2">
         <v>71</v>
@@ -6701,13 +6712,13 @@
         <v>71</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>161</v>
+        <v>193</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -6758,22 +6769,22 @@
         <v>71</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG48" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH48" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="AK48" t="s" s="2">
         <v>71</v>
@@ -6787,7 +6798,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6798,7 +6809,7 @@
         <v>72</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>71</v>
@@ -6810,13 +6821,13 @@
         <v>71</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -6867,22 +6878,22 @@
         <v>71</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH49" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>71</v>
@@ -6896,7 +6907,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6907,7 +6918,7 @@
         <v>72</v>
       </c>
       <c r="F50" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G50" t="s" s="2">
         <v>71</v>
@@ -6919,13 +6930,13 @@
         <v>71</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -6976,22 +6987,22 @@
         <v>71</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG50" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH50" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="AK50" t="s" s="2">
         <v>71</v>
@@ -7005,7 +7016,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7016,7 +7027,7 @@
         <v>72</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G51" t="s" s="2">
         <v>71</v>
@@ -7028,13 +7039,13 @@
         <v>71</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -7085,22 +7096,22 @@
         <v>71</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG51" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH51" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI51" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="AK51" t="s" s="2">
         <v>71</v>
@@ -7114,7 +7125,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7125,7 +7136,7 @@
         <v>72</v>
       </c>
       <c r="F52" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G52" t="s" s="2">
         <v>71</v>
@@ -7137,13 +7148,13 @@
         <v>71</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
@@ -7194,22 +7205,22 @@
         <v>71</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>72</v>
       </c>
       <c r="AG52" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH52" t="s" s="2">
         <v>71</v>
       </c>
       <c r="AI52" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AJ52" t="s" s="2">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="AK52" t="s" s="2">
         <v>71</v>

</xml_diff>